<commit_message>
Creacion tabla jFrame y arreglar errores
Logre ya lo de cargar el excel y que cuando se aprete la ventana de los sismos cargue la ventana, hice unos cambios para que funcionara y arregele unos errores
</commit_message>
<xml_diff>
--- a/Proyecto_Programado_1_POO/InformacionSismos.xlsx
+++ b/Proyecto_Programado_1_POO/InformacionSismos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCPC\Documents\NetBeansProjects\Proyecto_Programado_1_POO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32E859A-BF9D-45FD-905D-F47C687A935D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA91B456-EFE9-4395-9815-C4DE25F52AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA630437-BE34-4451-9ACC-A45962E560FA}"/>
   </bookViews>
@@ -34,40 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Fecha_Hora</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Magnitud</t>
-  </si>
-  <si>
-    <t>Profundidad</t>
-  </si>
-  <si>
-    <t>Origen</t>
-  </si>
-  <si>
-    <t>Latitud</t>
-  </si>
-  <si>
-    <t>Longitud</t>
-  </si>
-  <si>
-    <t>Localizacion</t>
-  </si>
-  <si>
-    <t>Provincia</t>
-  </si>
-  <si>
-    <t>Maritimo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
   <si>
     <t>Si</t>
   </si>
@@ -712,7 +679,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,670 +695,636 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1">
+        <v>200</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="1">
+        <v>10.1187</v>
+      </c>
+      <c r="H1" s="1">
+        <v>-84.161000000000001</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1">
-        <v>200</v>
+        <v>215</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1">
-        <v>10.1187</v>
+        <v>8.6359999999999992</v>
       </c>
       <c r="H2" s="1">
-        <v>-84.161000000000001</v>
+        <v>-82.930999999999997</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G3" s="1">
-        <v>8.6359999999999992</v>
+        <v>9.6487999999999996</v>
       </c>
       <c r="H3" s="1">
-        <v>-82.930999999999997</v>
+        <v>-84.034400000000005</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G4" s="1">
-        <v>9.6487999999999996</v>
+        <v>9.952</v>
       </c>
       <c r="H4" s="1">
-        <v>-84.034400000000005</v>
+        <v>-84.153999999999996</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E5" s="1">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G5" s="1">
-        <v>9.952</v>
+        <v>9.4558999999999997</v>
       </c>
       <c r="H5" s="1">
-        <v>-84.153999999999996</v>
+        <v>-85.392899999999997</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E6" s="1">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G6" s="1">
-        <v>9.4558999999999997</v>
+        <v>9.0180000000000007</v>
       </c>
       <c r="H6" s="1">
-        <v>-85.392899999999997</v>
+        <v>-83.668999999999997</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="E7" s="1">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1">
-        <v>9.0180000000000007</v>
+        <v>10.1647</v>
       </c>
       <c r="H7" s="1">
-        <v>-83.668999999999997</v>
+        <v>-83.7393</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1">
-        <v>10.1647</v>
+        <v>9.5079999999999991</v>
       </c>
       <c r="H8" s="1">
-        <v>-83.7393</v>
+        <v>-83.944999999999993</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G9" s="1">
-        <v>9.5079999999999991</v>
+        <v>9.8480000000000008</v>
       </c>
       <c r="H9" s="1">
-        <v>-83.944999999999993</v>
+        <v>-84.174999999999997</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G10" s="1">
-        <v>9.8480000000000008</v>
+        <v>9.65</v>
       </c>
       <c r="H10" s="1">
-        <v>-84.174999999999997</v>
+        <v>-84</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G11" s="1">
-        <v>9.65</v>
+        <v>8.5660000000000007</v>
       </c>
       <c r="H11" s="1">
-        <v>-84</v>
+        <v>-83.24</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1">
-        <v>350</v>
+        <v>365</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1">
-        <v>8.5660000000000007</v>
+        <v>9.6504999999999992</v>
       </c>
       <c r="H12" s="1">
-        <v>-83.24</v>
+        <v>-83.830399999999997</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1">
-        <v>365</v>
+        <v>380</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G13" s="1">
-        <v>9.6504999999999992</v>
+        <v>8.2432999999999996</v>
       </c>
       <c r="H13" s="1">
-        <v>-83.830399999999997</v>
+        <v>-83.033500000000004</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E14" s="1">
-        <v>380</v>
+        <v>395</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1">
-        <v>8.2432999999999996</v>
+        <v>9.4978999999999996</v>
       </c>
       <c r="H14" s="1">
-        <v>-83.033500000000004</v>
+        <v>-83.659099999999995</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1">
-        <v>395</v>
+        <v>410</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="G15" s="1">
-        <v>9.4978999999999996</v>
+        <v>10.5839</v>
       </c>
       <c r="H15" s="1">
-        <v>-83.659099999999995</v>
+        <v>-83.858400000000003</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1">
-        <v>410</v>
+        <v>425</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G16" s="1">
-        <v>10.5839</v>
+        <v>10.235799999999999</v>
       </c>
       <c r="H16" s="1">
-        <v>-83.858400000000003</v>
+        <v>-84.022800000000004</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1">
-        <v>425</v>
+        <v>440</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1">
-        <v>10.235799999999999</v>
+        <v>11.136100000000001</v>
       </c>
       <c r="H17" s="1">
-        <v>-84.022800000000004</v>
+        <v>-85.872200000000007</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="E18" s="1">
-        <v>440</v>
+        <v>455</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="G18" s="1">
-        <v>11.136100000000001</v>
+        <v>9.3163</v>
       </c>
       <c r="H18" s="1">
-        <v>-85.872200000000007</v>
+        <v>-83.950299999999999</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="1">
-        <v>455</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="1">
-        <v>9.3163</v>
-      </c>
-      <c r="H19" s="1">
-        <v>-83.950299999999999</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>